<commit_message>
Add LSTM, GAN to Note CS231n.xlsx
</commit_message>
<xml_diff>
--- a/CS231n.xlsx
+++ b/CS231n.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="4950" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="4950" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Overall process" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="Neural Networks" sheetId="6" r:id="rId5"/>
     <sheet name="CNN" sheetId="7" r:id="rId6"/>
     <sheet name="RNN" sheetId="8" r:id="rId7"/>
+    <sheet name="LSTM" sheetId="9" r:id="rId8"/>
+    <sheet name="GAN" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="154">
   <si>
     <t>i = 1,2,3,…,N</t>
   </si>
@@ -741,13 +743,34 @@
   <si>
     <t>W_proj (X, H)</t>
   </si>
+  <si>
+    <t>http://colah.github.io/posts/2015-08-Understanding-LSTMs/</t>
+  </si>
+  <si>
+    <t>Colah's blog</t>
+  </si>
+  <si>
+    <t>http://www.deeplearningbook.org/contents/rnn.html</t>
+  </si>
+  <si>
+    <t>Challenge of long term dependency (Ian Goodfellow's deep learning text book)</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1406.2661.pdf</t>
+  </si>
+  <si>
+    <t>Ian's GAN paper</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1701.00160.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -991,7 +1014,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -18157,8 +18180,8 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -18179,8 +18202,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4381500" y="7753350"/>
-          <a:ext cx="1104900" cy="1933575"/>
+          <a:off x="8039100" y="8896350"/>
+          <a:ext cx="1104900" cy="2000250"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -18543,8 +18566,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4429125" y="2524125"/>
-          <a:ext cx="1009650" cy="2705100"/>
+          <a:off x="8086725" y="3000375"/>
+          <a:ext cx="1009650" cy="2876550"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -18671,8 +18694,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4429125" y="5867400"/>
-          <a:ext cx="1009650" cy="1266825"/>
+          <a:off x="8086725" y="6515100"/>
+          <a:ext cx="1009650" cy="1295400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -19392,8 +19415,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -20983,15 +21006,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -21006,8 +21029,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1790701" y="7800975"/>
-          <a:ext cx="1104900" cy="828675"/>
+          <a:off x="1524000" y="7820025"/>
+          <a:ext cx="1371601" cy="1066800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -21046,7 +21069,34 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>CNN feature</a:t>
+            <a:t>CNN image</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>feature </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(N, X)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -21058,13 +21108,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>42863</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -21081,9 +21131,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2895601" y="8215313"/>
-          <a:ext cx="1457324" cy="57149"/>
+        <a:xfrm flipV="1">
+          <a:off x="2895601" y="8272462"/>
+          <a:ext cx="1457324" cy="80963"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
@@ -21249,6 +21299,1227 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>257176</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152398</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>361951</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="Group 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{380CBDF9-81AA-40B8-92B4-43033CE9FC7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="16106776" y="152398"/>
+          <a:ext cx="8172450" cy="5257801"/>
+          <a:chOff x="16106776" y="152398"/>
+          <a:chExt cx="8172450" cy="5257801"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle: Folded Corner 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCCA8DA9-1348-439F-97FE-DD9C2B1BF310}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16106776" y="152398"/>
+            <a:ext cx="8172450" cy="5257801"/>
+          </a:xfrm>
+          <a:prstGeom prst="foldedCorner">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 10221"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="de-DE" sz="2000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>熟读唐诗三百首，不会作诗也会吟</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" altLang="zh-CN" sz="2000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" altLang="zh-CN" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="de-DE" altLang="zh-CN" sz="1800">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Forward pass</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - word embedding (vocabulary table, vocabulary weight matrix)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - compute activation step by step (so called Recurrent NN)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - all nodes on the same layer share the same weight and bias</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - can be used for image captioning (CNN image features as h0)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - In image caption case, T is the longest caption in training samples</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - In common time series case, T is a fixed number, e.g. T=25</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>2) Backward pass</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - Update all weights and bias, including vocabulary weight matrix</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>3) Test (Sample)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - No need to do the recurrent computing as in the training phase</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>     - Always sample the word with largest probablity as the input of the next step</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="9" name="Picture 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087F6907-BABC-4515-820F-3F344F206101}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="17828170" y="647700"/>
+            <a:ext cx="3278982" cy="457165"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>225157</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>161267</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A84953C-30B3-4E39-8C0D-57F3523CFCF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7219950"/>
+          <a:ext cx="11807557" cy="5133317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>557199</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>119613</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F01B021-13A6-4364-97A8-D21907A53796}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10920399" y="9544051"/>
+          <a:ext cx="7777176" cy="4958312"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>8228</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Group 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C3C2699-EA8B-4AFC-B0A8-89C73B44BD4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="8477250"/>
+          <a:ext cx="10371428" cy="6647619"/>
+          <a:chOff x="0" y="8477250"/>
+          <a:chExt cx="10371428" cy="6647619"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="2" name="Picture 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3D993CD-8EB9-4431-AD4F-D02B3863F24D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="8477250"/>
+            <a:ext cx="10371428" cy="6647619"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Rectangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E4602A4-6FCB-42F2-B36A-79F9C5043357}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="28575" y="9896475"/>
+            <a:ext cx="10191750" cy="3848100"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00">
+              <a:alpha val="20000"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>560838</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0105FE24-B562-4C17-8DE2-E40CC416091A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1285875"/>
+          <a:ext cx="9095238" cy="1714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>513219</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66045</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="Group 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADA967A3-5BE9-4300-A703-D455220C256B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="2409825"/>
+          <a:ext cx="9047619" cy="5038095"/>
+          <a:chOff x="0" y="2409825"/>
+          <a:chExt cx="9047619" cy="5038095"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="7" name="Picture 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{406F9F34-B04A-42E1-94DE-28323C4E2CC2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="2409825"/>
+            <a:ext cx="9047619" cy="5038095"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Rectangle 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCACC7E5-F70F-4C48-B9FF-1D624C0AF72F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="38100" y="5448300"/>
+            <a:ext cx="8991600" cy="1962150"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00">
+              <a:alpha val="20000"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle: Folded Corner 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66FA5CB2-A060-464C-A976-7C0380135B49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10467975" y="3209925"/>
+          <a:ext cx="9067800" cy="4714875"/>
+        </a:xfrm>
+        <a:prstGeom prst="foldedCorner">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10221"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="de-DE" sz="2000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>十年生死两茫茫，不思量，自难忘</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" altLang="zh-CN" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" altLang="zh-CN" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Cell</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>     - only have simple linear addition, therefore not easy to lose long term info</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1800" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>2) Gates</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>     - f (forget gate): control whether to forget previous cell state</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>     - i (input gate): control whether to input previous h state to next cell state</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>     - g (input): control how much we would like to input previous h state into next cell state</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>     - o (output gate): control whether to use previous h state in the output for next h state</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1800" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>3) Get good empirical result. Did not see solid mathematics support.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1800" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>4) Check Andrej's blog to gain more intuition and explanation of LSTM</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1800">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>36800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>93948</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0965039-A6F8-4DA0-B546-3BB68DBCD7D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1057275"/>
+          <a:ext cx="10400000" cy="10419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E50516B3-7828-4CC6-AD87-FA94997FF294}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="3524250"/>
+          <a:ext cx="10125075" cy="1304925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00">
+            <a:alpha val="20000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>560457</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>56758</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3573DD8C-9B4B-43D0-9C4D-4FF82A7067E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="12115800"/>
+          <a:ext cx="12142857" cy="3133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>303755</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>180320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36AFD41F-3554-4149-BE58-F7CC9A4E9233}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12668250" y="11849100"/>
+          <a:ext cx="8361905" cy="5238095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>398899</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>122534</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661B5142-AFA0-4210-B3AE-C507BDEE0534}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10696575" y="990600"/>
+          <a:ext cx="9209524" cy="10323809"/>
+          <a:chOff x="10696575" y="990600"/>
+          <a:chExt cx="9209524" cy="10323809"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="6" name="Picture 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FD6A24E-813E-4209-BF1C-BA9311FFE295}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10696575" y="990600"/>
+            <a:ext cx="9209524" cy="10323809"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Rectangle 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD30B8C1-39DC-41CF-9135-1ABFA312E425}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11191876" y="10134600"/>
+            <a:ext cx="8096250" cy="1076325"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00">
+              <a:alpha val="20000"/>
+            </a:srgbClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -22254,8 +23525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AF33" sqref="AF33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22767,4 +24038,81 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <drawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AH46" sqref="AH46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A41" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A42" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>